<commit_message>
Oppdatert punktlighet for kollektivtransport
</commit_message>
<xml_diff>
--- a/Data/Mobilitet_i_Telemark/Buss_og_ferge/Punktlighet/RTI_HIST_DETAIL_REGION_LINJE_RAWT_092025.xlsx
+++ b/Data/Mobilitet_i_Telemark/Buss_og_ferge/Punktlighet/RTI_HIST_DETAIL_REGION_LINJE_RAWT_092025.xlsx
@@ -133,13 +133,13 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>952831.0</v>
+        <v>1050056.0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>441972.0</v>
+        <v>488560.0</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>510859.0</v>
+        <v>561496.0</v>
       </c>
     </row>
     <row r="4">
@@ -153,13 +153,13 @@
         <v>9.0</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>6381.0</v>
+        <v>6987.0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2369.0</v>
+        <v>2597.0</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>4012.0</v>
+        <v>4390.0</v>
       </c>
     </row>
     <row r="5">
@@ -173,13 +173,13 @@
         <v>9.0</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>4915.0</v>
+        <v>5390.0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1297.0</v>
+        <v>1467.0</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>3618.0</v>
+        <v>3923.0</v>
       </c>
     </row>
     <row r="6">
@@ -193,13 +193,13 @@
         <v>9.0</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>5876.0</v>
+        <v>6395.0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1417.0</v>
+        <v>1573.0</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>4459.0</v>
+        <v>4822.0</v>
       </c>
     </row>
     <row r="7">
@@ -213,13 +213,13 @@
         <v>9.0</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>5687.0</v>
+        <v>6207.0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2129.0</v>
+        <v>2299.0</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>3558.0</v>
+        <v>3908.0</v>
       </c>
     </row>
     <row r="8">
@@ -233,10 +233,10 @@
         <v>9.0</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>827.0</v>
+        <v>877.0</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>313.0</v>
+        <v>363.0</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>514.0</v>
@@ -253,13 +253,13 @@
         <v>9.0</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1666.0</v>
+        <v>1788.0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>252.0</v>
+        <v>309.0</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>1414.0</v>
+        <v>1479.0</v>
       </c>
     </row>
     <row r="10">
@@ -273,13 +273,13 @@
         <v>9.0</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>223190.0</v>
+        <v>246139.0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>109211.0</v>
+        <v>120119.0</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>113979.0</v>
+        <v>126020.0</v>
       </c>
     </row>
     <row r="11">
@@ -293,13 +293,13 @@
         <v>9.0</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>95797.0</v>
+        <v>105291.0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>51669.0</v>
+        <v>56895.0</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>44128.0</v>
+        <v>48396.0</v>
       </c>
     </row>
     <row r="12">
@@ -313,13 +313,13 @@
         <v>9.0</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>109706.0</v>
+        <v>120896.0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>53516.0</v>
+        <v>59158.0</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>56190.0</v>
+        <v>61738.0</v>
       </c>
     </row>
     <row r="13">
@@ -333,13 +333,13 @@
         <v>9.0</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>27231.0</v>
+        <v>30024.0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>17628.0</v>
+        <v>19411.0</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>9603.0</v>
+        <v>10613.0</v>
       </c>
     </row>
     <row r="14">
@@ -353,13 +353,13 @@
         <v>9.0</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>38123.0</v>
+        <v>41827.0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>24323.0</v>
+        <v>26653.0</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>13800.0</v>
+        <v>15174.0</v>
       </c>
     </row>
     <row r="15">
@@ -373,13 +373,13 @@
         <v>9.0</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>17349.0</v>
+        <v>19100.0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>6533.0</v>
+        <v>7144.0</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>10816.0</v>
+        <v>11956.0</v>
       </c>
     </row>
     <row r="16">
@@ -393,13 +393,13 @@
         <v>9.0</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>41535.0</v>
+        <v>45629.0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>14427.0</v>
+        <v>16117.0</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>27108.0</v>
+        <v>29512.0</v>
       </c>
     </row>
     <row r="17">
@@ -413,13 +413,13 @@
         <v>9.0</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>25984.0</v>
+        <v>28809.0</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>10906.0</v>
+        <v>12187.0</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>15078.0</v>
+        <v>16622.0</v>
       </c>
     </row>
     <row r="18">
@@ -433,13 +433,13 @@
         <v>9.0</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>13340.0</v>
+        <v>14753.0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>5823.0</v>
+        <v>6496.0</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>7517.0</v>
+        <v>8257.0</v>
       </c>
     </row>
     <row r="19">
@@ -453,13 +453,13 @@
         <v>9.0</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>14731.0</v>
+        <v>16437.0</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>8759.0</v>
+        <v>9854.0</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>5972.0</v>
+        <v>6583.0</v>
       </c>
     </row>
     <row r="20">
@@ -473,13 +473,13 @@
         <v>9.0</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>4365.0</v>
+        <v>4816.0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>2182.0</v>
+        <v>2413.0</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>2183.0</v>
+        <v>2403.0</v>
       </c>
     </row>
     <row r="21">
@@ -493,13 +493,13 @@
         <v>9.0</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>3537.0</v>
+        <v>3913.0</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>571.0</v>
+        <v>679.0</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>2966.0</v>
+        <v>3234.0</v>
       </c>
     </row>
     <row r="22">
@@ -513,13 +513,13 @@
         <v>9.0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>573.0</v>
+        <v>605.0</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>253.0</v>
+        <v>260.0</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>320.0</v>
+        <v>345.0</v>
       </c>
     </row>
     <row r="23">
@@ -533,13 +533,13 @@
         <v>9.0</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>7724.0</v>
+        <v>8593.0</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>4139.0</v>
+        <v>4670.0</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>3585.0</v>
+        <v>3923.0</v>
       </c>
     </row>
     <row r="24">
@@ -553,13 +553,13 @@
         <v>9.0</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>9163.0</v>
+        <v>10075.0</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>5136.0</v>
+        <v>5660.0</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>4027.0</v>
+        <v>4415.0</v>
       </c>
     </row>
     <row r="25">
@@ -573,13 +573,13 @@
         <v>9.0</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>504.0</v>
+        <v>535.0</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>86.0</v>
+        <v>90.0</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>418.0</v>
+        <v>445.0</v>
       </c>
     </row>
     <row r="26">
@@ -593,13 +593,13 @@
         <v>9.0</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>1732.0</v>
+        <v>1897.0</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>957.0</v>
+        <v>1056.0</v>
       </c>
       <c r="F26" s="3" t="n">
-        <v>775.0</v>
+        <v>841.0</v>
       </c>
     </row>
     <row r="27">
@@ -633,13 +633,13 @@
         <v>9.0</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>637.0</v>
+        <v>696.0</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>313.0</v>
+        <v>332.0</v>
       </c>
       <c r="F28" s="3" t="n">
-        <v>324.0</v>
+        <v>364.0</v>
       </c>
     </row>
     <row r="29">
@@ -653,13 +653,13 @@
         <v>9.0</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>642.0</v>
+        <v>1147.0</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>99.0</v>
+        <v>241.0</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>543.0</v>
+        <v>906.0</v>
       </c>
     </row>
     <row r="30">
@@ -673,13 +673,13 @@
         <v>9.0</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>177.0</v>
+        <v>195.0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>27.0</v>
+        <v>30.0</v>
       </c>
       <c r="F30" s="3" t="n">
-        <v>150.0</v>
+        <v>165.0</v>
       </c>
     </row>
     <row r="31">
@@ -693,13 +693,13 @@
         <v>9.0</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>966.0</v>
+        <v>1065.0</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>336.0</v>
+        <v>377.0</v>
       </c>
       <c r="F31" s="3" t="n">
-        <v>630.0</v>
+        <v>688.0</v>
       </c>
     </row>
     <row r="32">
@@ -713,13 +713,13 @@
         <v>9.0</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>674.0</v>
+        <v>745.0</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>137.0</v>
+        <v>141.0</v>
       </c>
       <c r="F32" s="3" t="n">
-        <v>537.0</v>
+        <v>604.0</v>
       </c>
     </row>
     <row r="33">
@@ -733,13 +733,13 @@
         <v>9.0</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>1364.0</v>
+        <v>1495.0</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>239.0</v>
+        <v>252.0</v>
       </c>
       <c r="F33" s="3" t="n">
-        <v>1125.0</v>
+        <v>1243.0</v>
       </c>
     </row>
     <row r="34">
@@ -753,13 +753,13 @@
         <v>9.0</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>1228.0</v>
+        <v>1360.0</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>196.0</v>
+        <v>238.0</v>
       </c>
       <c r="F34" s="3" t="n">
-        <v>1032.0</v>
+        <v>1122.0</v>
       </c>
     </row>
     <row r="35">
@@ -773,13 +773,13 @@
         <v>9.0</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>326.0</v>
+        <v>349.0</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>135.0</v>
+        <v>144.0</v>
       </c>
       <c r="F35" s="3" t="n">
-        <v>191.0</v>
+        <v>205.0</v>
       </c>
     </row>
     <row r="36">
@@ -793,13 +793,13 @@
         <v>9.0</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>574.0</v>
+        <v>628.0</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>472.0</v>
+        <v>520.0</v>
       </c>
       <c r="F36" s="3" t="n">
-        <v>102.0</v>
+        <v>108.0</v>
       </c>
     </row>
     <row r="37">
@@ -813,13 +813,13 @@
         <v>9.0</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>5376.0</v>
+        <v>5891.0</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>1904.0</v>
+        <v>2153.0</v>
       </c>
       <c r="F37" s="3" t="n">
-        <v>3472.0</v>
+        <v>3738.0</v>
       </c>
     </row>
     <row r="38">
@@ -833,13 +833,13 @@
         <v>9.0</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2201.0</v>
+        <v>2427.0</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>471.0</v>
+        <v>527.0</v>
       </c>
       <c r="F38" s="3" t="n">
-        <v>1730.0</v>
+        <v>1900.0</v>
       </c>
     </row>
     <row r="39">
@@ -853,13 +853,13 @@
         <v>9.0</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>1080.0</v>
+        <v>1173.0</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>205.0</v>
+        <v>216.0</v>
       </c>
       <c r="F39" s="3" t="n">
-        <v>875.0</v>
+        <v>957.0</v>
       </c>
     </row>
     <row r="40">
@@ -873,13 +873,13 @@
         <v>9.0</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>516.0</v>
+        <v>574.0</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>360.0</v>
+        <v>396.0</v>
       </c>
       <c r="F40" s="3" t="n">
-        <v>156.0</v>
+        <v>178.0</v>
       </c>
     </row>
     <row r="41">
@@ -893,13 +893,13 @@
         <v>9.0</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>560.0</v>
+        <v>615.0</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>106.0</v>
+        <v>118.0</v>
       </c>
       <c r="F41" s="3" t="n">
-        <v>454.0</v>
+        <v>497.0</v>
       </c>
     </row>
     <row r="42">
@@ -933,13 +933,13 @@
         <v>9.0</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>1620.0</v>
+        <v>1793.0</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>469.0</v>
+        <v>519.0</v>
       </c>
       <c r="F43" s="3" t="n">
-        <v>1151.0</v>
+        <v>1274.0</v>
       </c>
     </row>
     <row r="44">
@@ -953,13 +953,13 @@
         <v>9.0</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>1573.0</v>
+        <v>1694.0</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>263.0</v>
+        <v>298.0</v>
       </c>
       <c r="F44" s="3" t="n">
-        <v>1310.0</v>
+        <v>1396.0</v>
       </c>
     </row>
     <row r="45">
@@ -973,13 +973,13 @@
         <v>9.0</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>3144.0</v>
+        <v>3468.0</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>1449.0</v>
+        <v>1571.0</v>
       </c>
       <c r="F45" s="3" t="n">
-        <v>1695.0</v>
+        <v>1897.0</v>
       </c>
     </row>
     <row r="46">
@@ -993,13 +993,13 @@
         <v>9.0</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>841.0</v>
+        <v>929.0</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>198.0</v>
+        <v>215.0</v>
       </c>
       <c r="F46" s="3" t="n">
-        <v>643.0</v>
+        <v>714.0</v>
       </c>
     </row>
     <row r="47">
@@ -1013,13 +1013,13 @@
         <v>9.0</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>426.0</v>
+        <v>473.0</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>25.0</v>
+        <v>27.0</v>
       </c>
       <c r="F47" s="3" t="n">
-        <v>401.0</v>
+        <v>446.0</v>
       </c>
     </row>
     <row r="48">
@@ -1033,10 +1033,10 @@
         <v>9.0</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>294.0</v>
+        <v>329.0</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>286.0</v>
+        <v>321.0</v>
       </c>
       <c r="F48" s="3" t="n">
         <v>8.0</v>
@@ -1053,13 +1053,13 @@
         <v>9.0</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>71.0</v>
+        <v>83.0</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>26.0</v>
+        <v>30.0</v>
       </c>
       <c r="F49" s="3" t="n">
-        <v>45.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="50">
@@ -1073,13 +1073,13 @@
         <v>9.0</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>441.0</v>
+        <v>483.0</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>272.0</v>
+        <v>298.0</v>
       </c>
       <c r="F50" s="3" t="n">
-        <v>169.0</v>
+        <v>185.0</v>
       </c>
     </row>
     <row r="51">
@@ -1093,13 +1093,13 @@
         <v>9.0</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>1786.0</v>
+        <v>1976.0</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>697.0</v>
+        <v>784.0</v>
       </c>
       <c r="F51" s="3" t="n">
-        <v>1089.0</v>
+        <v>1192.0</v>
       </c>
     </row>
     <row r="52">
@@ -1113,13 +1113,13 @@
         <v>9.0</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>57588.0</v>
+        <v>63209.0</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>28305.0</v>
+        <v>30824.0</v>
       </c>
       <c r="F52" s="3" t="n">
-        <v>29283.0</v>
+        <v>32385.0</v>
       </c>
     </row>
     <row r="53">
@@ -1133,13 +1133,13 @@
         <v>9.0</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>24389.0</v>
+        <v>27192.0</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>13469.0</v>
+        <v>15086.0</v>
       </c>
       <c r="F53" s="3" t="n">
-        <v>10920.0</v>
+        <v>12106.0</v>
       </c>
     </row>
     <row r="54">
@@ -1153,13 +1153,13 @@
         <v>9.0</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>13304.0</v>
+        <v>14778.0</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>6630.0</v>
+        <v>7477.0</v>
       </c>
       <c r="F54" s="3" t="n">
-        <v>6674.0</v>
+        <v>7301.0</v>
       </c>
     </row>
     <row r="55">
@@ -1173,13 +1173,13 @@
         <v>9.0</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>737.0</v>
+        <v>758.0</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>281.0</v>
+        <v>287.0</v>
       </c>
       <c r="F55" s="3" t="n">
-        <v>456.0</v>
+        <v>471.0</v>
       </c>
     </row>
     <row r="56">
@@ -1193,13 +1193,13 @@
         <v>9.0</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>13597.0</v>
+        <v>14947.0</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>4392.0</v>
+        <v>4854.0</v>
       </c>
       <c r="F56" s="3" t="n">
-        <v>9205.0</v>
+        <v>10093.0</v>
       </c>
     </row>
     <row r="57">
@@ -1213,13 +1213,13 @@
         <v>9.0</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>5128.0</v>
+        <v>5625.0</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>1723.0</v>
+        <v>1846.0</v>
       </c>
       <c r="F57" s="3" t="n">
-        <v>3405.0</v>
+        <v>3779.0</v>
       </c>
     </row>
     <row r="58">
@@ -1233,13 +1233,13 @@
         <v>9.0</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>2142.0</v>
+        <v>2366.0</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>768.0</v>
+        <v>885.0</v>
       </c>
       <c r="F58" s="3" t="n">
-        <v>1374.0</v>
+        <v>1481.0</v>
       </c>
     </row>
     <row r="59">
@@ -1253,13 +1253,13 @@
         <v>9.0</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>555.0</v>
+        <v>601.0</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>94.0</v>
+        <v>105.0</v>
       </c>
       <c r="F59" s="3" t="n">
-        <v>461.0</v>
+        <v>496.0</v>
       </c>
     </row>
     <row r="60">
@@ -1273,13 +1273,13 @@
         <v>9.0</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>219.0</v>
+        <v>242.0</v>
       </c>
       <c r="E60" s="2" t="n">
         <v>7.0</v>
       </c>
       <c r="F60" s="3" t="n">
-        <v>212.0</v>
+        <v>235.0</v>
       </c>
     </row>
     <row r="61">
@@ -1293,13 +1293,13 @@
         <v>9.0</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>474.0</v>
+        <v>523.0</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>112.0</v>
+        <v>119.0</v>
       </c>
       <c r="F61" s="3" t="n">
-        <v>362.0</v>
+        <v>404.0</v>
       </c>
     </row>
     <row r="62">
@@ -1313,13 +1313,13 @@
         <v>9.0</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>2986.0</v>
+        <v>3320.0</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>1384.0</v>
+        <v>1540.0</v>
       </c>
       <c r="F62" s="3" t="n">
-        <v>1602.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="63">
@@ -1333,13 +1333,13 @@
         <v>9.0</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>18164.0</v>
+        <v>19747.0</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>5034.0</v>
+        <v>5433.0</v>
       </c>
       <c r="F63" s="3" t="n">
-        <v>13130.0</v>
+        <v>14314.0</v>
       </c>
     </row>
     <row r="64">
@@ -1353,13 +1353,13 @@
         <v>9.0</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>5144.0</v>
+        <v>5641.0</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>2187.0</v>
+        <v>2485.0</v>
       </c>
       <c r="F64" s="3" t="n">
-        <v>2957.0</v>
+        <v>3156.0</v>
       </c>
     </row>
     <row r="65">
@@ -1373,13 +1373,13 @@
         <v>9.0</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>6435.0</v>
+        <v>7087.0</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>2831.0</v>
+        <v>3180.0</v>
       </c>
       <c r="F65" s="3" t="n">
-        <v>3604.0</v>
+        <v>3907.0</v>
       </c>
     </row>
     <row r="66">
@@ -1393,13 +1393,13 @@
         <v>9.0</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>17693.0</v>
+        <v>19509.0</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>7681.0</v>
+        <v>8529.0</v>
       </c>
       <c r="F66" s="3" t="n">
-        <v>10012.0</v>
+        <v>10980.0</v>
       </c>
     </row>
     <row r="67">
@@ -1413,13 +1413,13 @@
         <v>9.0</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>430.0</v>
+        <v>474.0</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>122.0</v>
+        <v>132.0</v>
       </c>
       <c r="F67" s="3" t="n">
-        <v>308.0</v>
+        <v>342.0</v>
       </c>
     </row>
     <row r="68">
@@ -1433,13 +1433,13 @@
         <v>9.0</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>1703.0</v>
+        <v>1937.0</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>465.0</v>
+        <v>566.0</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>1238.0</v>
+        <v>1371.0</v>
       </c>
     </row>
     <row r="69">
@@ -1453,13 +1453,13 @@
         <v>9.0</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>469.0</v>
+        <v>517.0</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>64.0</v>
+        <v>68.0</v>
       </c>
       <c r="F69" s="3" t="n">
-        <v>405.0</v>
+        <v>449.0</v>
       </c>
     </row>
     <row r="70">
@@ -1473,13 +1473,13 @@
         <v>9.0</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>590.0</v>
+        <v>651.0</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>318.0</v>
+        <v>346.0</v>
       </c>
       <c r="F70" s="3" t="n">
-        <v>272.0</v>
+        <v>305.0</v>
       </c>
     </row>
     <row r="71">
@@ -1493,13 +1493,13 @@
         <v>9.0</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>2770.0</v>
+        <v>3096.0</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>1093.0</v>
+        <v>1196.0</v>
       </c>
       <c r="F71" s="3" t="n">
-        <v>1677.0</v>
+        <v>1900.0</v>
       </c>
     </row>
     <row r="72">
@@ -1513,13 +1513,13 @@
         <v>9.0</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>1919.0</v>
+        <v>2121.0</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>824.0</v>
+        <v>951.0</v>
       </c>
       <c r="F72" s="3" t="n">
-        <v>1095.0</v>
+        <v>1170.0</v>
       </c>
     </row>
     <row r="73">
@@ -1533,13 +1533,13 @@
         <v>9.0</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>188.0</v>
+        <v>213.0</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>45.0</v>
+        <v>57.0</v>
       </c>
       <c r="F73" s="3" t="n">
-        <v>143.0</v>
+        <v>156.0</v>
       </c>
     </row>
     <row r="74">
@@ -1553,13 +1553,13 @@
         <v>9.0</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>11623.0</v>
+        <v>12647.0</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>3266.0</v>
+        <v>3488.0</v>
       </c>
       <c r="F74" s="3" t="n">
-        <v>8357.0</v>
+        <v>9159.0</v>
       </c>
     </row>
     <row r="75">
@@ -1573,13 +1573,13 @@
         <v>9.0</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>355.0</v>
+        <v>389.0</v>
       </c>
       <c r="E75" s="2" t="n">
         <v>17.0</v>
       </c>
       <c r="F75" s="3" t="n">
-        <v>338.0</v>
+        <v>372.0</v>
       </c>
     </row>
     <row r="76">
@@ -1593,13 +1593,13 @@
         <v>9.0</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>103.0</v>
+        <v>113.0</v>
       </c>
       <c r="E76" s="2" t="n">
         <v>24.0</v>
       </c>
       <c r="F76" s="3" t="n">
-        <v>79.0</v>
+        <v>89.0</v>
       </c>
     </row>
     <row r="77">
@@ -1613,13 +1613,13 @@
         <v>9.0</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>8097.0</v>
+        <v>8797.0</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>4679.0</v>
+        <v>5153.0</v>
       </c>
       <c r="F77" s="3" t="n">
-        <v>3418.0</v>
+        <v>3644.0</v>
       </c>
     </row>
     <row r="78">
@@ -1633,13 +1633,13 @@
         <v>9.0</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>959.0</v>
+        <v>1106.0</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>312.0</v>
+        <v>376.0</v>
       </c>
       <c r="F78" s="3" t="n">
-        <v>647.0</v>
+        <v>730.0</v>
       </c>
     </row>
     <row r="79">
@@ -1653,13 +1653,13 @@
         <v>9.0</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>3225.0</v>
+        <v>3516.0</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>1289.0</v>
+        <v>1421.0</v>
       </c>
       <c r="F79" s="3" t="n">
-        <v>1936.0</v>
+        <v>2095.0</v>
       </c>
     </row>
     <row r="80">
@@ -1673,13 +1673,13 @@
         <v>9.0</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>149.0</v>
+        <v>168.0</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="F80" s="3" t="n">
-        <v>109.0</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="81">
@@ -1693,13 +1693,13 @@
         <v>9.0</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>808.0</v>
+        <v>924.0</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>197.0</v>
+        <v>241.0</v>
       </c>
       <c r="F81" s="3" t="n">
-        <v>611.0</v>
+        <v>683.0</v>
       </c>
     </row>
     <row r="82">
@@ -1713,13 +1713,13 @@
         <v>9.0</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>11924.0</v>
+        <v>13080.0</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>4920.0</v>
+        <v>5629.0</v>
       </c>
       <c r="F82" s="3" t="n">
-        <v>7004.0</v>
+        <v>7451.0</v>
       </c>
     </row>
     <row r="83">
@@ -1733,13 +1733,13 @@
         <v>9.0</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>13001.0</v>
+        <v>14534.0</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>2614.0</v>
+        <v>3023.0</v>
       </c>
       <c r="F83" s="3" t="n">
-        <v>10387.0</v>
+        <v>11511.0</v>
       </c>
     </row>
     <row r="84">
@@ -1753,13 +1753,13 @@
         <v>9.0</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>315.0</v>
+        <v>359.0</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>61.0</v>
+        <v>68.0</v>
       </c>
       <c r="F84" s="3" t="n">
-        <v>254.0</v>
+        <v>291.0</v>
       </c>
     </row>
     <row r="85">
@@ -1773,13 +1773,13 @@
         <v>9.0</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>2555.0</v>
+        <v>2855.0</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>424.0</v>
+        <v>500.0</v>
       </c>
       <c r="F85" s="3" t="n">
-        <v>2131.0</v>
+        <v>2355.0</v>
       </c>
     </row>
     <row r="86">
@@ -1793,13 +1793,13 @@
         <v>9.0</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>409.0</v>
+        <v>452.0</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>103.0</v>
+        <v>117.0</v>
       </c>
       <c r="F86" s="3" t="n">
-        <v>306.0</v>
+        <v>335.0</v>
       </c>
     </row>
     <row r="87">
@@ -1813,13 +1813,13 @@
         <v>9.0</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>963.0</v>
+        <v>1077.0</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>192.0</v>
+        <v>206.0</v>
       </c>
       <c r="F87" s="3" t="n">
-        <v>771.0</v>
+        <v>871.0</v>
       </c>
     </row>
     <row r="88">
@@ -1833,13 +1833,13 @@
         <v>9.0</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>469.0</v>
+        <v>521.0</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>251.0</v>
+        <v>293.0</v>
       </c>
       <c r="F88" s="3" t="n">
-        <v>218.0</v>
+        <v>228.0</v>
       </c>
     </row>
     <row r="89">
@@ -1853,13 +1853,13 @@
         <v>9.0</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>1232.0</v>
+        <v>1383.0</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>301.0</v>
+        <v>385.0</v>
       </c>
       <c r="F89" s="3" t="n">
-        <v>931.0</v>
+        <v>998.0</v>
       </c>
     </row>
     <row r="90">
@@ -1873,13 +1873,13 @@
         <v>9.0</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>704.0</v>
+        <v>786.0</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>111.0</v>
+        <v>123.0</v>
       </c>
       <c r="F90" s="3" t="n">
-        <v>593.0</v>
+        <v>663.0</v>
       </c>
     </row>
     <row r="91">
@@ -1893,13 +1893,13 @@
         <v>9.0</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>969.0</v>
+        <v>1062.0</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>640.0</v>
+        <v>705.0</v>
       </c>
       <c r="F91" s="3" t="n">
-        <v>329.0</v>
+        <v>357.0</v>
       </c>
     </row>
     <row r="92">
@@ -1913,13 +1913,13 @@
         <v>9.0</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>1338.0</v>
+        <v>1466.0</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>324.0</v>
+        <v>382.0</v>
       </c>
       <c r="F92" s="3" t="n">
-        <v>1014.0</v>
+        <v>1084.0</v>
       </c>
     </row>
     <row r="93">
@@ -1933,13 +1933,13 @@
         <v>9.0</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>735.0</v>
+        <v>814.0</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>357.0</v>
+        <v>402.0</v>
       </c>
       <c r="F93" s="3" t="n">
-        <v>378.0</v>
+        <v>412.0</v>
       </c>
     </row>
     <row r="94">
@@ -1953,13 +1953,13 @@
         <v>9.0</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>441.0</v>
+        <v>487.0</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>181.0</v>
+        <v>213.0</v>
       </c>
       <c r="F94" s="3" t="n">
-        <v>260.0</v>
+        <v>274.0</v>
       </c>
     </row>
     <row r="95">
@@ -1973,10 +1973,10 @@
         <v>9.0</v>
       </c>
       <c r="D95" s="1" t="n">
-        <v>114.0</v>
+        <v>142.0</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>85.0</v>
+        <v>113.0</v>
       </c>
       <c r="F95" s="3" t="n">
         <v>29.0</v>
@@ -2013,13 +2013,13 @@
         <v>9.0</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>79.0</v>
+        <v>84.0</v>
       </c>
       <c r="E97" s="2" t="n">
         <v>9.0</v>
       </c>
       <c r="F97" s="3" t="n">
-        <v>70.0</v>
+        <v>75.0</v>
       </c>
     </row>
     <row r="98">
@@ -2033,13 +2033,13 @@
         <v>9.0</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>795.0</v>
+        <v>890.0</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>596.0</v>
+        <v>649.0</v>
       </c>
       <c r="F98" s="3" t="n">
-        <v>199.0</v>
+        <v>241.0</v>
       </c>
     </row>
     <row r="99">
@@ -2053,13 +2053,13 @@
         <v>9.0</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>388.0</v>
+        <v>430.0</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>165.0</v>
+        <v>183.0</v>
       </c>
       <c r="F99" s="3" t="n">
-        <v>223.0</v>
+        <v>247.0</v>
       </c>
     </row>
     <row r="100">
@@ -2073,13 +2073,13 @@
         <v>9.0</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>430.0</v>
+        <v>481.0</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>184.0</v>
+        <v>224.0</v>
       </c>
       <c r="F100" s="3" t="n">
-        <v>246.0</v>
+        <v>257.0</v>
       </c>
     </row>
     <row r="101">
@@ -2093,13 +2093,13 @@
         <v>9.0</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>943.0</v>
+        <v>1041.0</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>152.0</v>
+        <v>180.0</v>
       </c>
       <c r="F101" s="3" t="n">
-        <v>791.0</v>
+        <v>861.0</v>
       </c>
     </row>
     <row r="102">
@@ -2113,13 +2113,13 @@
         <v>9.0</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>987.0</v>
+        <v>1080.0</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>425.0</v>
+        <v>482.0</v>
       </c>
       <c r="F102" s="3" t="n">
-        <v>562.0</v>
+        <v>598.0</v>
       </c>
     </row>
     <row r="103">
@@ -2133,13 +2133,13 @@
         <v>9.0</v>
       </c>
       <c r="D103" s="1" t="n">
-        <v>261.0</v>
+        <v>310.0</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>194.0</v>
+        <v>229.0</v>
       </c>
       <c r="F103" s="3" t="n">
-        <v>67.0</v>
+        <v>81.0</v>
       </c>
     </row>
     <row r="104">
@@ -2153,13 +2153,13 @@
         <v>9.0</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>1295.0</v>
+        <v>1413.0</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>429.0</v>
+        <v>456.0</v>
       </c>
       <c r="F104" s="3" t="n">
-        <v>866.0</v>
+        <v>957.0</v>
       </c>
     </row>
     <row r="105">
@@ -2173,13 +2173,13 @@
         <v>9.0</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>6657.0</v>
+        <v>7308.0</v>
       </c>
       <c r="E105" s="2" t="n">
-        <v>2951.0</v>
+        <v>3207.0</v>
       </c>
       <c r="F105" s="3" t="n">
-        <v>3706.0</v>
+        <v>4101.0</v>
       </c>
     </row>
     <row r="106">
@@ -2193,13 +2193,13 @@
         <v>9.0</v>
       </c>
       <c r="D106" s="1" t="n">
-        <v>5353.0</v>
+        <v>5896.0</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>1435.0</v>
+        <v>1535.0</v>
       </c>
       <c r="F106" s="3" t="n">
-        <v>3918.0</v>
+        <v>4361.0</v>
       </c>
     </row>
     <row r="107">
@@ -2213,13 +2213,13 @@
         <v>9.0</v>
       </c>
       <c r="D107" s="1" t="n">
-        <v>534.0</v>
+        <v>587.0</v>
       </c>
       <c r="E107" s="2" t="n">
-        <v>125.0</v>
+        <v>153.0</v>
       </c>
       <c r="F107" s="3" t="n">
-        <v>409.0</v>
+        <v>434.0</v>
       </c>
     </row>
     <row r="108">
@@ -2233,13 +2233,13 @@
         <v>9.0</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>1043.0</v>
+        <v>1153.0</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>549.0</v>
+        <v>626.0</v>
       </c>
       <c r="F108" s="3" t="n">
-        <v>494.0</v>
+        <v>527.0</v>
       </c>
     </row>
     <row r="109">
@@ -2253,13 +2253,13 @@
         <v>9.0</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>767.0</v>
+        <v>843.0</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>118.0</v>
+        <v>154.0</v>
       </c>
       <c r="F109" s="3" t="n">
-        <v>649.0</v>
+        <v>689.0</v>
       </c>
     </row>
     <row r="110">
@@ -2273,13 +2273,13 @@
         <v>9.0</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>1118.0</v>
+        <v>1229.0</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>481.0</v>
+        <v>524.0</v>
       </c>
       <c r="F110" s="3" t="n">
-        <v>637.0</v>
+        <v>705.0</v>
       </c>
     </row>
     <row r="111">
@@ -2293,13 +2293,13 @@
         <v>9.0</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>922.0</v>
+        <v>1002.0</v>
       </c>
       <c r="E111" s="2" t="n">
-        <v>590.0</v>
+        <v>656.0</v>
       </c>
       <c r="F111" s="3" t="n">
-        <v>332.0</v>
+        <v>346.0</v>
       </c>
     </row>
     <row r="112">
@@ -2313,13 +2313,13 @@
         <v>9.0</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>1095.0</v>
+        <v>1191.0</v>
       </c>
       <c r="E112" s="2" t="n">
-        <v>297.0</v>
+        <v>320.0</v>
       </c>
       <c r="F112" s="3" t="n">
-        <v>798.0</v>
+        <v>871.0</v>
       </c>
     </row>
     <row r="113">
@@ -2333,13 +2333,13 @@
         <v>9.0</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>826.0</v>
+        <v>939.0</v>
       </c>
       <c r="E113" s="2" t="n">
-        <v>246.0</v>
+        <v>324.0</v>
       </c>
       <c r="F113" s="3" t="n">
-        <v>580.0</v>
+        <v>615.0</v>
       </c>
     </row>
     <row r="114">
@@ -2353,13 +2353,13 @@
         <v>9.0</v>
       </c>
       <c r="D114" s="1" t="n">
-        <v>1050.0</v>
+        <v>1141.0</v>
       </c>
       <c r="E114" s="2" t="n">
-        <v>588.0</v>
+        <v>647.0</v>
       </c>
       <c r="F114" s="3" t="n">
-        <v>462.0</v>
+        <v>494.0</v>
       </c>
     </row>
     <row r="115">
@@ -2373,13 +2373,13 @@
         <v>9.0</v>
       </c>
       <c r="D115" s="1" t="n">
-        <v>2451.0</v>
+        <v>2678.0</v>
       </c>
       <c r="E115" s="2" t="n">
-        <v>1015.0</v>
+        <v>1108.0</v>
       </c>
       <c r="F115" s="3" t="n">
-        <v>1436.0</v>
+        <v>1570.0</v>
       </c>
     </row>
     <row r="116">
@@ -2393,13 +2393,13 @@
         <v>9.0</v>
       </c>
       <c r="D116" s="1" t="n">
-        <v>725.0</v>
+        <v>882.0</v>
       </c>
       <c r="E116" s="2" t="n">
-        <v>141.0</v>
+        <v>217.0</v>
       </c>
       <c r="F116" s="3" t="n">
-        <v>584.0</v>
+        <v>665.0</v>
       </c>
     </row>
     <row r="117">
@@ -2413,13 +2413,13 @@
         <v>9.0</v>
       </c>
       <c r="D117" s="1" t="n">
-        <v>826.0</v>
+        <v>954.0</v>
       </c>
       <c r="E117" s="2" t="n">
-        <v>203.0</v>
+        <v>280.0</v>
       </c>
       <c r="F117" s="3" t="n">
-        <v>623.0</v>
+        <v>674.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>